<commit_message>
fixing ops and expo errors
</commit_message>
<xml_diff>
--- a/Experiments/exp_treatment_info.xlsx
+++ b/Experiments/exp_treatment_info.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="2200" windowWidth="25600" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="0" windowWidth="25600" windowHeight="16960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
   <si>
     <t>Site</t>
   </si>
@@ -70,6 +73,42 @@
   </si>
   <si>
     <t>clarkduke</t>
+  </si>
+  <si>
+    <t>bace</t>
+  </si>
+  <si>
+    <t>temptreat_units</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Watts</t>
+  </si>
+  <si>
+    <t>preciptreat_1</t>
+  </si>
+  <si>
+    <t>preciptreat_-1</t>
+  </si>
+  <si>
+    <t>preciptreat_units</t>
+  </si>
+  <si>
+    <t>perc</t>
+  </si>
+  <si>
+    <t>rmbl</t>
+  </si>
+  <si>
+    <t>chuine</t>
+  </si>
+  <si>
+    <t>jasper</t>
+  </si>
+  <si>
+    <t>oklahoma</t>
   </si>
 </sst>
 </file>
@@ -83,11 +122,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -104,6 +138,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,31 +162,1248 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0946968821236515"/>
+          <c:y val="0.070631970260223"/>
+          <c:w val="0.785984121626308"/>
+          <c:h val="0.732342007434944"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>T</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FCF305"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FFFF00"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]graphs!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]graphs!$D$5:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>T+</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF9900"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]graphs!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]graphs!$G$5:$G$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>T++</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="DD0806"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DD0806"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="DD0806"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]graphs!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]graphs!$J$5:$J$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>H</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="0000D4"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="3366FF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="0000D4"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]graphs!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]graphs!$K$5:$K$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>S</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="00ABEA"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00ABEA"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="00ABEA"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>[1]graphs!$A$5:$A$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]graphs!$L$5:$L$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1812389624"/>
+        <c:axId val="1812386488"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="1812389624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="925" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1812386488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="14.0"/>
+        <c:majorTimeUnit val="days"/>
+        <c:minorUnit val="7.0"/>
+        <c:minorTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1812386488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="10.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="3175">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="3175">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="925" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+                <a:ea typeface="Arial"/>
+                <a:cs typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1812389624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="C0C0C0"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.895832504889744"/>
+          <c:y val="0.323420074349442"/>
+          <c:w val="0.0909090068387055"/>
+          <c:h val="0.226765799256506"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="C0C0C0"/>
+        </a:solidFill>
+        <a:ln w="3175">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:ea typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="3175">
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="925" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial"/>
+          <a:ea typeface="Arial"/>
+          <a:cs typeface="Arial"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.4921259845" footer="0.4921259845"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="graphs"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,15 +1728,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="13" max="13" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,16 +1759,28 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -528,17 +1799,29 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="L2">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -557,17 +1840,29 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -586,17 +1881,29 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -615,19 +1922,93 @@
       <c r="F5" t="s">
         <v>3</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>200</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>150</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>